<commit_message>
Ajuste para envio de e-mail
</commit_message>
<xml_diff>
--- a/cots.xlsx
+++ b/cots.xlsx
@@ -8,44 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72ce4925f28c6d35/EstudosHeroku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_2B078027D83192EFDA81B552EFA4D3433381407C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F18C4A33-B214-40DC-BF92-651B634B7882}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_2B078027D83192EFDA81B552EFA4D3433381407C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60ACB38E-80E3-4A05-BB3A-603E881AFB3C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Data/Hora</t>
-  </si>
-  <si>
-    <t>Dolar</t>
-  </si>
-  <si>
-    <t>Euro</t>
-  </si>
-  <si>
-    <t>Bitcoin</t>
-  </si>
-  <si>
-    <t>2022-06-17 16:56:19.694356</t>
-  </si>
-  <si>
-    <t>5.1428</t>
-  </si>
-  <si>
-    <t>5.3969</t>
-  </si>
-  <si>
-    <t>106.04</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,46 +406,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>